<commit_message>
Brand Page + catelogyPage+ productPage+ dashboardPage
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/logindata.xlsx
+++ b/src/test/resources/testdata/logindata.xlsx
@@ -3,22 +3,24 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tester\Automation\SeleniumTesstNG_Parallel\src\test\resources\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tester\Automation\Hoa_Baitapcuoikhoa_AT04\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC2839E8-B879-44EE-97E6-ADDA86F6C23C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4E47E8B-119B-4A8B-8AB5-0CA4C8A952FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14205" yWindow="4215" windowWidth="14595" windowHeight="11385" xr2:uid="{6A5B7545-1E47-48FC-9C01-3B596E42F566}"/>
+    <workbookView xWindow="2385" yWindow="4095" windowWidth="14595" windowHeight="11385" activeTab="2" xr2:uid="{6A5B7545-1E47-48FC-9C01-3B596E42F566}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Login" sheetId="1" r:id="rId1"/>
+    <sheet name="Category" sheetId="2" r:id="rId2"/>
+    <sheet name="Product" sheetId="3" r:id="rId3"/>
+    <sheet name="Brand" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="50">
   <si>
     <t>email</t>
   </si>
@@ -66,14 +68,135 @@
     <t>fail</t>
   </si>
   <si>
-    <t>pass</t>
+    <t>Name Brand</t>
+  </si>
+  <si>
+    <t>Title Brand</t>
+  </si>
+  <si>
+    <t>Description Brand</t>
+  </si>
+  <si>
+    <t>Zara</t>
+  </si>
+  <si>
+    <t>Zara logo – Thương hiệu thời trang nổi tiếng thế giới</t>
+  </si>
+  <si>
+    <t>Đặt khách hàng làm trọng tâm khi thiết kế sản phẩm là một trong những yếu tố góp phần làm nên thành công của thương hiệu đình đám Zara.
+Nhắc đến Zara hẳn rất nhiều người sẽ nhớ đến thương hiệu bán lẻ thời trang nổi tiếng thế giới. Với việc tạo ra một đế chế thời trang bán lẻ phát triển nhanh chóng, Zara khao khát tạo ra niềm đam mê với thời trang giữa nhiều người tiêu dùng, trải khắp các nền văn hóa và nhóm tuổi khác nhau.
+Zara được Amancio Ortega và Rosalía Mera thành lập vào năm 1975 ở thành phố Galicia, Tây Ban Nha. Cửa hàng đầu tiên bày bán đồ quần áo có giá rẻ. Và trong vòng 8 năm sau đó, cách tiếp cận thời trang và mô hình kinh doanh của Zara dần tạo ra sức hút với người tiêu dùng Tây Ban Nha cùng với đó là 9 cửa hàng được mở mới tại các thành phố lớn nhất của Tây Ban Nha.</t>
+  </si>
+  <si>
+    <t>TinNgoan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WILL YOU BE MINE FOREVER? </t>
+  </si>
+  <si>
+    <t>Là địa chỉ quen thuộc của các KOLs Việt, Tingoan cung cấp nhiều mẫu váy áo đa dạng, từ váy liền, áo crop top, quần short, chân váy đến giày dép.</t>
+  </si>
+  <si>
+    <t>Product Name</t>
+  </si>
+  <si>
+    <t>Kem nền</t>
+  </si>
+  <si>
+    <t>Túi xách</t>
+  </si>
+  <si>
+    <t>Category Name</t>
+  </si>
+  <si>
+    <t>Mỹ phẩm</t>
+  </si>
+  <si>
+    <t>Phụ kiện thời trang</t>
+  </si>
+  <si>
+    <t>Trang sức</t>
+  </si>
+  <si>
+    <t>ParentCategory</t>
+  </si>
+  <si>
+    <t>OrderingNumber</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>My Pham</t>
+  </si>
+  <si>
+    <t>Chanel</t>
+  </si>
+  <si>
+    <t>Hàng xách tay cao cấp</t>
+  </si>
+  <si>
+    <t>Dior</t>
+  </si>
+  <si>
+    <t>Phu Kien</t>
+  </si>
+  <si>
+    <t>Trang suc</t>
+  </si>
+  <si>
+    <t>PNJ</t>
+  </si>
+  <si>
+    <t>Hàng nhập khẩu Đức</t>
+  </si>
+  <si>
+    <t>Trang sức tinh tế</t>
+  </si>
+  <si>
+    <t>Brand Name</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>$</t>
+  </si>
+  <si>
+    <t>VND</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>Purchase</t>
+  </si>
+  <si>
+    <t>Tag</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>Unit Price</t>
+  </si>
+  <si>
+    <t>Discount</t>
+  </si>
+  <si>
+    <t>Quantity</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -91,18 +214,15 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill/>
-    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -110,15 +230,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -458,23 +602,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22A8E667-CD08-463E-96E3-F4C7BECAB2A0}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -482,13 +626,13 @@
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="0">
+      <c r="B2">
         <v>123456</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -496,13 +640,13 @@
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="0">
+      <c r="B3">
         <v>123457</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="D3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -517,28 +661,253 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86BA7726-BAE9-41E5-9960-212205C7140D}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s" s="0">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s" s="0">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="D2" t="s" s="2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2">
+        <v>1000</v>
+      </c>
+      <c r="D2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3">
+        <v>1011</v>
+      </c>
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4">
+        <v>1021</v>
+      </c>
+      <c r="D4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9C9991A-1CF2-4C86-9909-9978E5D69B76}">
+  <dimension ref="A1:J3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J1" sqref="B1:J1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2">
+        <v>0.8</v>
+      </c>
+      <c r="F2">
+        <v>200</v>
+      </c>
+      <c r="G2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H2">
+        <v>4000</v>
+      </c>
+      <c r="I2">
+        <v>300</v>
+      </c>
+      <c r="J2">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3">
+        <v>3.2</v>
+      </c>
+      <c r="F3">
+        <v>500</v>
+      </c>
+      <c r="G3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H3">
+        <v>5000</v>
+      </c>
+      <c r="I3">
+        <v>200</v>
+      </c>
+      <c r="J3">
+        <v>4000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED375110-64F6-490E-AD76-C9E3105BBAC6}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="2" max="2" width="41.5703125" customWidth="1"/>
+    <col min="3" max="3" width="84.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>9</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="4" customFormat="1" ht="195" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Search Product check Table (cột tên)
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/logindata.xlsx
+++ b/src/test/resources/testdata/logindata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tester\Automation\Hoa_Baitapcuoikhoa_AT04\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4E47E8B-119B-4A8B-8AB5-0CA4C8A952FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97B111EE-B97F-436F-9F2E-E28F8FCED427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2385" yWindow="4095" windowWidth="14595" windowHeight="11385" activeTab="2" xr2:uid="{6A5B7545-1E47-48FC-9C01-3B596E42F566}"/>
+    <workbookView xWindow="1080" yWindow="4215" windowWidth="14595" windowHeight="11385" activeTab="2" xr2:uid="{6A5B7545-1E47-48FC-9C01-3B596E42F566}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -130,9 +130,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>My Pham</t>
-  </si>
-  <si>
     <t>Chanel</t>
   </si>
   <si>
@@ -142,12 +139,6 @@
     <t>Dior</t>
   </si>
   <si>
-    <t>Phu Kien</t>
-  </si>
-  <si>
-    <t>Trang suc</t>
-  </si>
-  <si>
     <t>PNJ</t>
   </si>
   <si>
@@ -191,6 +182,15 @@
   </si>
   <si>
     <t>Quantity</t>
+  </si>
+  <si>
+    <t>Category 1</t>
+  </si>
+  <si>
+    <t>Mỹ Phẩm</t>
+  </si>
+  <si>
+    <t>Cake</t>
   </si>
 </sst>
 </file>
@@ -664,7 +664,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -696,16 +696,16 @@
         <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="C2">
         <v>1000</v>
       </c>
       <c r="D2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" t="s">
         <v>30</v>
-      </c>
-      <c r="E2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -713,16 +713,16 @@
         <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="C3">
         <v>1011</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -730,16 +730,16 @@
         <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="C4">
         <v>1021</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -752,7 +752,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="B1:J1"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -768,28 +768,28 @@
         <v>21</v>
       </c>
       <c r="C1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" t="s">
         <v>39</v>
       </c>
-      <c r="E1" t="s">
-        <v>42</v>
-      </c>
       <c r="F1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" t="s">
         <v>44</v>
       </c>
-      <c r="H1" t="s">
-        <v>47</v>
-      </c>
       <c r="I1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="J1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -797,13 +797,13 @@
         <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E2">
         <v>0.8</v>
@@ -812,7 +812,7 @@
         <v>200</v>
       </c>
       <c r="G2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="H2">
         <v>4000</v>
@@ -829,13 +829,13 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E3">
         <v>3.2</v>
@@ -844,7 +844,7 @@
         <v>500</v>
       </c>
       <c r="G3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H3">
         <v>5000</v>
@@ -866,8 +866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED375110-64F6-490E-AD76-C9E3105BBAC6}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>